<commit_message>
Actualizar Descrição de caso de uso
Criação de mais dois casos de uso 30 minutos os 3 elementos
</commit_message>
<xml_diff>
--- a/descricao de caso de uso.xlsx
+++ b/descricao de caso de uso.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis_\Documents\escola\es2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis_\Documents\GitHub\Engenharia-software-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="7965" xr2:uid="{35FA8BB6-F6EB-4A21-803F-1FFA0D7B92E9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="7965" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Folha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Escolher inquerito" sheetId="1" r:id="rId1"/>
+    <sheet name="Criar Trilho" sheetId="2" r:id="rId2"/>
+    <sheet name="Alterar trilho" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="53">
   <si>
     <t>nome</t>
   </si>
@@ -117,13 +119,79 @@
   </si>
   <si>
     <t>nenhum</t>
+  </si>
+  <si>
+    <t>Caso de Uso</t>
+  </si>
+  <si>
+    <t>Criar trilho</t>
+  </si>
+  <si>
+    <t>o ator vai criar um trilho</t>
+  </si>
+  <si>
+    <t>clicar no botão criar trilho</t>
+  </si>
+  <si>
+    <t>o sistema devolve um formulario com os dados a preencher</t>
+  </si>
+  <si>
+    <t>o ator preenche os dados do formulario e clica no botao criar</t>
+  </si>
+  <si>
+    <t>o sistema devolve um mensagem de sucesso</t>
+  </si>
+  <si>
+    <t>não está autorizado a criar trilhos</t>
+  </si>
+  <si>
+    <t>2.a</t>
+  </si>
+  <si>
+    <t>não devolveu o formulario</t>
+  </si>
+  <si>
+    <t>verificar se o sistema devolve o formulario</t>
+  </si>
+  <si>
+    <t>verificar se o ator consegue introduzir dados nos campos</t>
+  </si>
+  <si>
+    <t>verificar se o sistema devolve a mensagem de sucesso</t>
+  </si>
+  <si>
+    <t>o sistema devolve uma mensagem de erro de introdução de dados</t>
+  </si>
+  <si>
+    <t>Alterar trilho</t>
+  </si>
+  <si>
+    <t>o ator vai alterar um trilho</t>
+  </si>
+  <si>
+    <t>selecionar um trilho</t>
+  </si>
+  <si>
+    <t>clicar no botão Alterar trilho</t>
+  </si>
+  <si>
+    <t>o sistema devolve um formulario com os dados do trilho</t>
+  </si>
+  <si>
+    <t>o ator altera os dados do formulario desejados e clica no botao alterar</t>
+  </si>
+  <si>
+    <t>não está autorizado a alterar trilhos</t>
+  </si>
+  <si>
+    <t>o sistema devolve uma mensagem de erro na alteração de dados</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,16 +199,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -148,12 +229,115 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,163 +651,572 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B1D5248-9D10-4CBE-B366-F69B6BF34CFE}">
-  <dimension ref="A2:B23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:2" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="7"/>
+    </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>2</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>3</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>4</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+    </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+    </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="4" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>